<commit_message>
Atualiza arquivos com coluna padronizada NM_MUN
</commit_message>
<xml_diff>
--- a/dados/geoses_norte.xlsx
+++ b/dados/geoses_norte.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dd803c46cce71088/Documentos/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{61781E4E-4B3B-4697-B85E-BCEF08C76F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47C2F602-CCDE-421E-A5B7-00B950160CF5}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{215F98E9-DA76-4162-9E8D-7B88262A397B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="450">
   <si>
-    <t>municipio</t>
-  </si>
-  <si>
     <t>GeoSES</t>
   </si>
   <si>
@@ -1375,12 +1366,15 @@
   </si>
   <si>
     <t>Xambioá</t>
+  </si>
+  <si>
+    <t>NM_MUN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1733,18 +1727,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8802DD7-649B-416D-AD92-55E0E43C9747}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B451"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1755,15 +1749,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" s="1">
         <v>-0.32493209645195598</v>
@@ -1771,7 +1765,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="1">
         <v>-0.31506741185226</v>
@@ -1779,7 +1773,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B4" s="1">
         <v>-0.31678320280666999</v>
@@ -1787,7 +1781,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="1">
         <v>-0.75164660072471201</v>
@@ -1795,7 +1789,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1">
         <v>-0.47466817179714299</v>
@@ -1803,7 +1797,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="1">
         <v>-0.87542970593798297</v>
@@ -1811,7 +1805,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8" s="1">
         <v>-0.37091262576275402</v>
@@ -1819,7 +1813,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B9" s="1">
         <v>-0.29973287240857499</v>
@@ -1827,7 +1821,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10" s="1">
         <v>-0.67546632798809803</v>
@@ -1835,7 +1829,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B11" s="1">
         <v>-0.31368914765422901</v>
@@ -1843,7 +1837,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B12" s="1">
         <v>-0.47643010449220702</v>
@@ -1851,7 +1845,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B13" s="1">
         <v>-0.27306648004690398</v>
@@ -1859,7 +1853,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B14" s="1">
         <v>-0.40244166091871703</v>
@@ -1867,7 +1861,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B15" s="1">
         <v>-6.4572585392635704E-2</v>
@@ -1875,7 +1869,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B16" s="1">
         <v>-0.70919004466125202</v>
@@ -1883,7 +1877,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B17" s="1">
         <v>-0.821345193212766</v>
@@ -1891,7 +1885,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B18" s="1">
         <v>-0.358173139369868</v>
@@ -1899,7 +1893,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1">
         <v>-0.71514705924854405</v>
@@ -1907,7 +1901,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B20" s="1">
         <v>0.215798255045937</v>
@@ -1915,7 +1909,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B21" s="1">
         <v>-0.49008178220065901</v>
@@ -1923,7 +1917,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B22" s="1">
         <v>-1</v>
@@ -1931,7 +1925,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1">
         <v>0.15582175146722799</v>
@@ -1939,7 +1933,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="1">
         <v>-0.89944421527301699</v>
@@ -1947,7 +1941,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B25" s="1">
         <v>-0.81041842150142196</v>
@@ -1955,7 +1949,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" s="1">
         <v>-0.43056438386568402</v>
@@ -1963,7 +1957,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B27" s="1">
         <v>-0.206843771045889</v>
@@ -1971,7 +1965,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B28" s="1">
         <v>0.36918825074742501</v>
@@ -1979,7 +1973,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B29" s="1">
         <v>-0.55868280817237703</v>
@@ -1987,7 +1981,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B30" s="1">
         <v>-0.50724907730262303</v>
@@ -1995,7 +1989,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" s="1">
         <v>-0.58020918619324602</v>
@@ -2003,7 +1997,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B32" s="1">
         <v>-0.36613972894977098</v>
@@ -2011,7 +2005,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B33" s="1">
         <v>-0.22158173360345201</v>
@@ -2019,7 +2013,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B34" s="1">
         <v>-0.49553347145823201</v>
@@ -2027,7 +2021,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B35" s="1">
         <v>-0.54473519303795404</v>
@@ -2035,7 +2029,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B36" s="1">
         <v>-2.1039205649162299E-2</v>
@@ -2043,7 +2037,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B37" s="1">
         <v>0.53450087764113396</v>
@@ -2051,7 +2045,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B38" s="1">
         <v>-0.46900718202060399</v>
@@ -2059,7 +2053,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B39" s="1">
         <v>-0.43887334580892701</v>
@@ -2067,7 +2061,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B40" s="1">
         <v>-0.12884025407202301</v>
@@ -2075,7 +2069,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B41" s="1">
         <v>0.46881610801527701</v>
@@ -2083,7 +2077,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B42" s="1">
         <v>-0.45325700499885402</v>
@@ -2091,7 +2085,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B43" s="1">
         <v>-0.45352850732892402</v>
@@ -2099,7 +2093,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" s="1">
         <v>-0.90340305939381704</v>
@@ -2107,7 +2101,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B45" s="1">
         <v>-0.25898764084667503</v>
@@ -2115,7 +2109,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B46" s="1">
         <v>-0.77837496919025295</v>
@@ -2123,7 +2117,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B47" s="1">
         <v>-0.55066499440236905</v>
@@ -2131,7 +2125,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B48" s="1">
         <v>-0.32016732781475699</v>
@@ -2139,7 +2133,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B49" s="1">
         <v>-0.66716071406723398</v>
@@ -2147,7 +2141,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B50" s="1">
         <v>-0.84270677030747798</v>
@@ -2155,7 +2149,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B51" s="1">
         <v>-0.45979976043578802</v>
@@ -2163,7 +2157,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B52" s="1">
         <v>-0.29543288821814701</v>
@@ -2171,7 +2165,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B53" s="1">
         <v>-0.83976001917877097</v>
@@ -2179,7 +2173,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B54" s="1">
         <v>-0.57184062393929402</v>
@@ -2187,7 +2181,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B55" s="1">
         <v>-0.54026861171496798</v>
@@ -2195,7 +2189,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B56" s="1">
         <v>-0.31462252005916502</v>
@@ -2203,7 +2197,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B57" s="1">
         <v>-4.5156506611293099E-2</v>
@@ -2211,7 +2205,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B58" s="1">
         <v>-0.66512441126480404</v>
@@ -2219,7 +2213,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B59" s="1">
         <v>-0.59957531170449296</v>
@@ -2227,7 +2221,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B60" s="1">
         <v>-0.79072014066930796</v>
@@ -2235,7 +2229,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B61" s="1">
         <v>-0.33001690515481302</v>
@@ -2243,7 +2237,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B62" s="1">
         <v>1</v>
@@ -2251,7 +2245,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B63" s="1">
         <v>-0.57302674647680796</v>
@@ -2259,7 +2253,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B64" s="1">
         <v>-0.12086847978642801</v>
@@ -2267,7 +2261,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B65" s="1">
         <v>-0.63224829548741401</v>
@@ -2275,7 +2269,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B66" s="1">
         <v>-0.30903580454666002</v>
@@ -2283,7 +2277,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B67" s="1">
         <v>-0.83238396859737696</v>
@@ -2291,7 +2285,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B68" s="1">
         <v>1</v>
@@ -2299,7 +2293,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B69" s="1">
         <v>-0.70531696512786402</v>
@@ -2307,7 +2301,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B70" s="1">
         <v>-0.45801673172201501</v>
@@ -2315,7 +2309,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B71" s="1">
         <v>-0.38284472535674502</v>
@@ -2323,7 +2317,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B72" s="1">
         <v>-0.33440144856896198</v>
@@ -2331,7 +2325,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B73" s="1">
         <v>-0.34835688815870702</v>
@@ -2339,7 +2333,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B74" s="1">
         <v>-0.62002396975711205</v>
@@ -2347,7 +2341,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B75" s="1">
         <v>-0.727432067403324</v>
@@ -2355,7 +2349,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B76" s="1">
         <v>-0.34904833434087001</v>
@@ -2363,7 +2357,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B77" s="1">
         <v>-0.38060467934166498</v>
@@ -2371,7 +2365,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B78" s="1">
         <v>-0.27835807095794102</v>
@@ -2379,7 +2373,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B79" s="1">
         <v>-0.25958798022068902</v>
@@ -2387,7 +2381,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B80" s="1">
         <v>-0.38331386448326499</v>
@@ -2395,7 +2389,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B81" s="1">
         <v>-0.41630487938229799</v>
@@ -2403,7 +2397,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B82" s="1">
         <v>-0.51616822593365996</v>
@@ -2411,7 +2405,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B83" s="1">
         <v>-0.67341745840707601</v>
@@ -2419,7 +2413,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B84" s="1">
         <v>-0.46491091927189498</v>
@@ -2427,7 +2421,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B85" s="1">
         <v>-0.70110137170629205</v>
@@ -2435,7 +2429,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B86" s="1">
         <v>-0.460982050522035</v>
@@ -2443,7 +2437,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B87" s="1">
         <v>-0.35411010551022898</v>
@@ -2451,7 +2445,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B88" s="1">
         <v>-0.57017113049841295</v>
@@ -2459,7 +2453,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B89" s="1">
         <v>-0.50829980909250005</v>
@@ -2467,7 +2461,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B90" s="1">
         <v>-0.59310280612947197</v>
@@ -2475,7 +2469,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B91" s="1">
         <v>-0.92552090859823699</v>
@@ -2483,7 +2477,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B92" s="1">
         <v>-0.70362096391790796</v>
@@ -2491,7 +2485,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B93" s="1">
         <v>-0.46599472462618402</v>
@@ -2499,7 +2493,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B94" s="1">
         <v>0.52650042991360202</v>
@@ -2507,7 +2501,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B95" s="1">
         <v>-0.52920574199066694</v>
@@ -2515,7 +2509,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B96" s="1">
         <v>-0.47748672245994001</v>
@@ -2523,7 +2517,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B97" s="1">
         <v>-1</v>
@@ -2531,7 +2525,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B98" s="1">
         <v>-0.82631921530202201</v>
@@ -2539,7 +2533,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B99" s="1">
         <v>8.1533075789490705E-2</v>
@@ -2547,7 +2541,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B100" s="1">
         <v>-0.23877338535933701</v>
@@ -2555,7 +2549,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B101" s="1">
         <v>-0.36226292773132901</v>
@@ -2563,7 +2557,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B102" s="1">
         <v>-0.58453791422804402</v>
@@ -2571,7 +2565,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B103" s="1">
         <v>-0.14338911391638001</v>
@@ -2579,7 +2573,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B104" s="1">
         <v>-0.62298681412760004</v>
@@ -2587,7 +2581,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B105" s="1">
         <v>-0.475576656662129</v>
@@ -2595,7 +2589,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B106" s="1">
         <v>-7.43106932674516E-2</v>
@@ -2603,7 +2597,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B107" s="1">
         <v>-0.65462641432708601</v>
@@ -2611,7 +2605,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B108" s="1">
         <v>-0.60928715192875305</v>
@@ -2619,7 +2613,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B109" s="1">
         <v>-0.62672399950288704</v>
@@ -2627,7 +2621,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B110" s="1">
         <v>-0.17989739574725899</v>
@@ -2635,7 +2629,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B111" s="1">
         <v>-0.29904578670459497</v>
@@ -2643,7 +2637,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B112" s="1">
         <v>-0.25981523536854301</v>
@@ -2651,7 +2645,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B113" s="1">
         <v>-0.71261858033890002</v>
@@ -2659,7 +2653,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B114" s="1">
         <v>-0.34398096367599801</v>
@@ -2667,7 +2661,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B115" s="1">
         <v>8.4942327379012195E-2</v>
@@ -2675,7 +2669,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B116" s="1">
         <v>-0.59500618359785595</v>
@@ -2683,7 +2677,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B117" s="1">
         <v>-0.76769314745307304</v>
@@ -2691,7 +2685,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B118" s="1">
         <v>0.118943864136925</v>
@@ -2699,7 +2693,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B119" s="1">
         <v>-0.61765955340610601</v>
@@ -2707,7 +2701,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B120" s="1">
         <v>-0.44830704420157302</v>
@@ -2715,7 +2709,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B121" s="1">
         <v>-0.94033491562071403</v>
@@ -2723,7 +2717,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B122" s="1">
         <v>-0.35732943436706999</v>
@@ -2731,7 +2725,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B123" s="1">
         <v>-0.365664744497256</v>
@@ -2739,7 +2733,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B124" s="1">
         <v>-0.57980493825813995</v>
@@ -2747,7 +2741,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B125" s="1">
         <v>-0.50221909392326503</v>
@@ -2755,7 +2749,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B126" s="1">
         <v>0.13288156236641899</v>
@@ -2763,7 +2757,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B127" s="1">
         <v>-0.166566561243811</v>
@@ -2771,7 +2765,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B128" s="1">
         <v>-5.63666864378881E-2</v>
@@ -2779,7 +2773,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B129" s="1">
         <v>-0.14487169436766301</v>
@@ -2787,7 +2781,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B130" s="1">
         <v>-9.6940148251319594E-2</v>
@@ -2795,7 +2789,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B131" s="1">
         <v>-0.67996096808778805</v>
@@ -2803,7 +2797,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B132" s="1">
         <v>-0.50304514316000604</v>
@@ -2811,7 +2805,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B133" s="1">
         <v>-0.76714866167246298</v>
@@ -2819,7 +2813,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B134" s="1">
         <v>-0.81422639014583698</v>
@@ -2827,7 +2821,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B135" s="1">
         <v>-0.50753544080973201</v>
@@ -2835,7 +2829,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B136" s="1">
         <v>-5.8634372180411003E-2</v>
@@ -2843,7 +2837,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B137" s="1">
         <v>-0.33486024380444002</v>
@@ -2851,7 +2845,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B138" s="1">
         <v>-5.0726287761919397E-2</v>
@@ -2859,7 +2853,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B139" s="1">
         <v>-0.45083881907735102</v>
@@ -2867,7 +2861,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B140" s="1">
         <v>-0.533778540405077</v>
@@ -2875,7 +2869,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B141" s="1">
         <v>-0.32891756680845702</v>
@@ -2883,7 +2877,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B142" s="1">
         <v>-0.79184888362796901</v>
@@ -2891,7 +2885,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B143" s="1">
         <v>-0.70421761854979004</v>
@@ -2899,7 +2893,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B144" s="1">
         <v>-0.55911104645572995</v>
@@ -2907,7 +2901,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B145" s="1">
         <v>-0.28108824645399499</v>
@@ -2915,7 +2909,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B146" s="1">
         <v>-0.58690305277744903</v>
@@ -2923,7 +2917,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B147" s="1">
         <v>5.0452908870288696E-3</v>
@@ -2931,7 +2925,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B148" s="1">
         <v>-0.15829078473300501</v>
@@ -2939,7 +2933,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B149" s="1">
         <v>-0.58935638930191403</v>
@@ -2947,7 +2941,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B150" s="1">
         <v>-0.26004592083440198</v>
@@ -2955,7 +2949,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B151" s="1">
         <v>-0.24574440706849901</v>
@@ -2963,7 +2957,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B152" s="1">
         <v>-0.67431378404844899</v>
@@ -2971,7 +2965,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B153" s="1">
         <v>-0.53445426442931199</v>
@@ -2979,7 +2973,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B154" s="1">
         <v>-0.71197708887829703</v>
@@ -2987,7 +2981,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B155" s="1">
         <v>-3.8055897375026099E-2</v>
@@ -2995,7 +2989,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B156" s="1">
         <v>-0.95649725008045805</v>
@@ -3003,7 +2997,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B157" s="1">
         <v>1.9137998655571E-2</v>
@@ -3011,7 +3005,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B158" s="1">
         <v>-0.64986509416927396</v>
@@ -3019,7 +3013,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B159" s="1">
         <v>1.6204202438202302E-2</v>
@@ -3027,7 +3021,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B160" s="1">
         <v>-0.62560910982846396</v>
@@ -3035,7 +3029,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B161" s="1">
         <v>-0.61249502353458196</v>
@@ -3043,7 +3037,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B162" s="1">
         <v>-0.3</v>
@@ -3051,7 +3045,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B163" s="1">
         <v>-0.53289884557915701</v>
@@ -3059,7 +3053,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B164" s="1">
         <v>-0.483292593047085</v>
@@ -3067,7 +3061,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B165" s="1">
         <v>-0.79454226338822898</v>
@@ -3075,7 +3069,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B166" s="1">
         <v>-0.123607299415608</v>
@@ -3083,7 +3077,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B167" s="1">
         <v>-0.69318461739012205</v>
@@ -3091,7 +3085,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B168" s="1">
         <v>-0.39710060062876201</v>
@@ -3099,7 +3093,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B169" s="1">
         <v>-0.48126524965922701</v>
@@ -3107,7 +3101,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B170" s="1">
         <v>-0.77257686378266499</v>
@@ -3115,7 +3109,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B171" s="1">
         <v>-0.81837657788465001</v>
@@ -3123,7 +3117,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B172" s="1">
         <v>-0.63992437762112897</v>
@@ -3131,7 +3125,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B173" s="1">
         <v>-0.17735339529351299</v>
@@ -3139,7 +3133,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B174" s="1">
         <v>0.44897884188087001</v>
@@ -3147,7 +3141,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B175" s="1">
         <v>-0.71182849884233501</v>
@@ -3155,7 +3149,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B176" s="1">
         <v>0.67733984871632102</v>
@@ -3163,7 +3157,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B177" s="1">
         <v>-0.27198249240714401</v>
@@ -3171,7 +3165,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B178" s="1">
         <v>-0.34764833469425799</v>
@@ -3179,7 +3173,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B179" s="1">
         <v>-0.62361625410042598</v>
@@ -3187,7 +3181,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B180" s="1">
         <v>-0.53156760626467203</v>
@@ -3195,7 +3189,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B181" s="1">
         <v>-0.73062053687148398</v>
@@ -3203,7 +3197,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B182" s="1">
         <v>-0.75015157484703798</v>
@@ -3211,7 +3205,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B183" s="1">
         <v>-0.59407399781181103</v>
@@ -3219,7 +3213,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B184" s="1">
         <v>-0.50810343533374303</v>
@@ -3227,7 +3221,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B185" s="1">
         <v>-0.38006697124048899</v>
@@ -3235,7 +3229,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B186" s="1">
         <v>-0.61856918708578701</v>
@@ -3243,7 +3237,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B187" s="1">
         <v>-0.52482772599184302</v>
@@ -3251,7 +3245,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B188" s="1">
         <v>-0.12922982255712501</v>
@@ -3259,7 +3253,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B189" s="1">
         <v>-0.64121305472718804</v>
@@ -3267,7 +3261,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B190" s="1">
         <v>-7.8688342609430903E-2</v>
@@ -3275,7 +3269,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B191" s="1">
         <v>-0.984510450216601</v>
@@ -3283,7 +3277,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B192" s="1">
         <v>-0.24483772334732901</v>
@@ -3291,7 +3285,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B193" s="1">
         <v>-0.60656008199258005</v>
@@ -3299,7 +3293,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B194" s="1">
         <v>-0.19544721032145601</v>
@@ -3307,7 +3301,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B195" s="1">
         <v>-0.68465305763470496</v>
@@ -3315,7 +3309,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B196" s="1">
         <v>-0.57301780396640001</v>
@@ -3323,7 +3317,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B197" s="1">
         <v>-0.63955832432904902</v>
@@ -3331,7 +3325,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B198" s="1">
         <v>-0.53703065928327898</v>
@@ -3339,7 +3333,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B199" s="1">
         <v>-0.142146700181769</v>
@@ -3347,7 +3341,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B200" s="1">
         <v>-0.61896980119675504</v>
@@ -3355,7 +3349,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B201" s="1">
         <v>5.9298359185481798E-2</v>
@@ -3363,7 +3357,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B202" s="1">
         <v>-0.24196187471759401</v>
@@ -3371,7 +3365,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B203" s="1">
         <v>0.65488895305833095</v>
@@ -3379,7 +3373,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B204" s="1">
         <v>-1</v>
@@ -3387,7 +3381,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B205" s="1">
         <v>-0.55155499853970902</v>
@@ -3395,7 +3389,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B206" s="1">
         <v>-0.79850206962864301</v>
@@ -3403,7 +3397,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B207" s="1">
         <v>-0.53559962141936301</v>
@@ -3411,7 +3405,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B208" s="1">
         <v>-0.728668264072178</v>
@@ -3419,7 +3413,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B209" s="1">
         <v>-0.68787873395529997</v>
@@ -3427,7 +3421,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B210" s="1">
         <v>-0.153824822751537</v>
@@ -3435,7 +3429,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B211" s="1">
         <v>-0.76175511535681395</v>
@@ -3443,7 +3437,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B212" s="1">
         <v>-0.338197967053601</v>
@@ -3451,7 +3445,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B213" s="1">
         <v>-0.27267559099565603</v>
@@ -3459,7 +3453,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B214" s="1">
         <v>-0.34584104199655802</v>
@@ -3467,7 +3461,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B215" s="1">
         <v>-0.71800684255938496</v>
@@ -3475,7 +3469,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B216" s="1">
         <v>-0.84095849749770302</v>
@@ -3483,7 +3477,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B217" s="1">
         <v>-0.45679670907998399</v>
@@ -3491,7 +3485,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B218" s="1">
         <v>-0.99819183876040896</v>
@@ -3499,7 +3493,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B219" s="1">
         <v>-0.67594087429384198</v>
@@ -3507,7 +3501,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B220" s="1">
         <v>-0.26254419928084199</v>
@@ -3515,7 +3509,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B221" s="1">
         <v>-0.51169211323532904</v>
@@ -3523,7 +3517,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B222" s="1">
         <v>-0.21500937828348901</v>
@@ -3531,7 +3525,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B223" s="1">
         <v>-0.71210984915994402</v>
@@ -3539,7 +3533,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B224" s="1">
         <v>1</v>
@@ -3547,7 +3541,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B225" s="1">
         <v>-0.48898179820355597</v>
@@ -3555,7 +3549,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B226" s="1">
         <v>-0.42088201683632798</v>
@@ -3563,7 +3557,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B227" s="1">
         <v>-0.59592171910944602</v>
@@ -3571,7 +3565,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B228" s="1">
         <v>-0.86639307831536905</v>
@@ -3579,7 +3573,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B229" s="1">
         <v>9.5567833010680794E-2</v>
@@ -3587,7 +3581,7 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B230" s="1">
         <v>-0.58817518175262495</v>
@@ -3595,7 +3589,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B231" s="1">
         <v>-0.32781893827688102</v>
@@ -3603,7 +3597,7 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B232" s="1">
         <v>-0.95739558884669596</v>
@@ -3611,7 +3605,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B233" s="1">
         <v>-0.19937669061654001</v>
@@ -3619,7 +3613,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B234" s="1">
         <v>-3.0794181377269501E-2</v>
@@ -3627,7 +3621,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B235" s="1">
         <v>-0.65914750448259696</v>
@@ -3635,7 +3629,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B236" s="1">
         <v>-0.613959949598338</v>
@@ -3643,7 +3637,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B237" s="1">
         <v>-0.67570136959340199</v>
@@ -3651,7 +3645,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B238" s="1">
         <v>-0.17987404639929</v>
@@ -3659,7 +3653,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B239" s="1">
         <v>-0.43628190915970499</v>
@@ -3667,7 +3661,7 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B240" s="1">
         <v>-0.6</v>
@@ -3675,7 +3669,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B241" s="1">
         <v>-0.29517971541566701</v>
@@ -3683,7 +3677,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B242" s="1">
         <v>3.8023459427810997E-2</v>
@@ -3691,7 +3685,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B243" s="1">
         <v>-0.16033401517247001</v>
@@ -3699,7 +3693,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B244" s="1">
         <v>-0.57721066742946903</v>
@@ -3707,7 +3701,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B245" s="1">
         <v>-1</v>
@@ -3715,7 +3709,7 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B246" s="1">
         <v>-0.56512883010544301</v>
@@ -3723,7 +3717,7 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B247" s="1">
         <v>-0.58077540504214598</v>
@@ -3731,7 +3725,7 @@
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B248" s="1">
         <v>-0.484595181566432</v>
@@ -3739,7 +3733,7 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B249" s="1">
         <v>-0.56419294542945198</v>
@@ -3747,7 +3741,7 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B250" s="1">
         <v>-0.19198303592368199</v>
@@ -3755,7 +3749,7 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B251" s="1">
         <v>-0.35472042720901098</v>
@@ -3763,7 +3757,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B252" s="1">
         <v>-0.68989848101877804</v>
@@ -3771,7 +3765,7 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B253" s="1">
         <v>-0.17749859461148901</v>
@@ -3779,7 +3773,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B254" s="1">
         <v>-0.76359042141601396</v>
@@ -3787,7 +3781,7 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B255" s="1">
         <v>-0.33263841443074499</v>
@@ -3795,7 +3789,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B256" s="1">
         <v>-0.47215218976519402</v>
@@ -3803,7 +3797,7 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B257" s="1">
         <v>-0.69878322289976502</v>
@@ -3811,7 +3805,7 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B258" s="1">
         <v>-0.71356997327059501</v>
@@ -3819,7 +3813,7 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B259" s="1">
         <v>-0.43952969368494599</v>
@@ -3827,7 +3821,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B260" s="1">
         <v>-0.77656716250665603</v>
@@ -3835,7 +3829,7 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B261" s="1">
         <v>-0.513605306040815</v>
@@ -3843,7 +3837,7 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B262" s="1">
         <v>-0.67516167123755599</v>
@@ -3851,7 +3845,7 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B263" s="1">
         <v>-0.32151759224283999</v>
@@ -3859,7 +3853,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B264" s="1">
         <v>-0.647810228371964</v>
@@ -3867,7 +3861,7 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B265" s="1">
         <v>-0.38841462394346499</v>
@@ -3875,7 +3869,7 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B266" s="1">
         <v>-0.41565559422812598</v>
@@ -3883,7 +3877,7 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B267" s="1">
         <v>-0.85186428773384004</v>
@@ -3891,7 +3885,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B268" s="1">
         <v>-0.37306089948626397</v>
@@ -3899,7 +3893,7 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B269" s="1">
         <v>-0.482499653688721</v>
@@ -3907,7 +3901,7 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B270" s="1">
         <v>-0.122487230315499</v>
@@ -3915,7 +3909,7 @@
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B271" s="1">
         <v>-0.62712952263550603</v>
@@ -3923,7 +3917,7 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B272" s="1">
         <v>-0.87356124582823402</v>
@@ -3931,7 +3925,7 @@
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B273" s="1">
         <v>-0.65839376199461297</v>
@@ -3939,7 +3933,7 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B274" s="1">
         <v>0.34305847972734899</v>
@@ -3947,7 +3941,7 @@
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B275" s="1">
         <v>-0.48860163214841001</v>
@@ -3955,7 +3949,7 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B276" s="1">
         <v>-0.53005249496407703</v>
@@ -3963,7 +3957,7 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B277" s="1">
         <v>-0.59942699926663401</v>
@@ -3971,7 +3965,7 @@
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B278" s="1">
         <v>1</v>
@@ -3979,7 +3973,7 @@
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B279" s="1">
         <v>-0.14787443220511401</v>
@@ -3987,7 +3981,7 @@
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B280" s="1">
         <v>-0.46960157299621202</v>
@@ -3995,7 +3989,7 @@
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B281" s="1">
         <v>-0.42943649469766798</v>
@@ -4003,7 +3997,7 @@
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B282" s="1">
         <v>-2.4365764028866301E-4</v>
@@ -4011,7 +4005,7 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B283" s="1">
         <v>0.148843129380102</v>
@@ -4019,7 +4013,7 @@
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B284" s="1">
         <v>-0.65166443250122397</v>
@@ -4027,7 +4021,7 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B285" s="1">
         <v>-0.185577729259325</v>
@@ -4035,7 +4029,7 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B286" s="1">
         <v>-0.51503340599021696</v>
@@ -4043,7 +4037,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B287" s="1">
         <v>1</v>
@@ -4051,7 +4045,7 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B288" s="1">
         <v>-0.70867471370489399</v>
@@ -4059,7 +4053,7 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B289" s="1">
         <v>-0.45085772933500801</v>
@@ -4067,7 +4061,7 @@
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B290" s="1">
         <v>-5.5941932463385797E-3</v>
@@ -4075,7 +4069,7 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B291" s="1">
         <v>4.0121914636534799E-2</v>
@@ -4083,7 +4077,7 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B292" s="1">
         <v>0.60186347435659404</v>
@@ -4091,7 +4085,7 @@
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B293" s="1">
         <v>-0.84414550281557299</v>
@@ -4099,7 +4093,7 @@
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B294" s="1">
         <v>0.23162160928843001</v>
@@ -4107,7 +4101,7 @@
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B295" s="1">
         <v>-0.75062059059435904</v>
@@ -4115,7 +4109,7 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B296" s="1">
         <v>-0.17906129736168899</v>
@@ -4123,7 +4117,7 @@
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B297" s="1">
         <v>-0.43352859490280998</v>
@@ -4131,7 +4125,7 @@
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B298" s="1">
         <v>-0.320743099965694</v>
@@ -4139,7 +4133,7 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B299" s="1">
         <v>-0.78991602704785202</v>
@@ -4147,7 +4141,7 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B300" s="1">
         <v>-0.66819763842097402</v>
@@ -4155,7 +4149,7 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B301" s="1">
         <v>0.232298773267998</v>
@@ -4163,7 +4157,7 @@
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B302" s="1">
         <v>-0.258227429447899</v>
@@ -4171,7 +4165,7 @@
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B303" s="1">
         <v>-0.42952723876707699</v>
@@ -4179,7 +4173,7 @@
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B304" s="1">
         <v>-0.45847627222926701</v>
@@ -4187,7 +4181,7 @@
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B305" s="1">
         <v>-0.47547256210403499</v>
@@ -4195,7 +4189,7 @@
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B306" s="1">
         <v>0.43741037704680602</v>
@@ -4203,7 +4197,7 @@
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B307" s="1">
         <v>-0.77783563496863595</v>
@@ -4211,7 +4205,7 @@
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B308" s="1">
         <v>-0.55911246460936304</v>
@@ -4219,7 +4213,7 @@
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B309" s="1">
         <v>-0.462216137488485</v>
@@ -4227,7 +4221,7 @@
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B310" s="1">
         <v>-0.30791983597823402</v>
@@ -4235,7 +4229,7 @@
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B311" s="1">
         <v>-0.65163004259696</v>
@@ -4243,7 +4237,7 @@
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B312" s="1">
         <v>-0.20588536111318001</v>
@@ -4251,7 +4245,7 @@
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B313" s="1">
         <v>-0.60578630081106799</v>
@@ -4259,7 +4253,7 @@
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B314" s="1">
         <v>-0.71437498772541896</v>
@@ -4267,7 +4261,7 @@
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B315" s="1">
         <v>-0.43707126274221197</v>
@@ -4275,7 +4269,7 @@
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B316" s="1">
         <v>-0.68913289199656502</v>
@@ -4283,7 +4277,7 @@
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B317" s="1">
         <v>-0.52530189286572604</v>
@@ -4291,7 +4285,7 @@
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B318" s="1">
         <v>-0.52606128436181898</v>
@@ -4299,7 +4293,7 @@
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B319" s="1">
         <v>-0.70824035542325803</v>
@@ -4307,7 +4301,7 @@
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B320" s="1">
         <v>5.5104605788376997E-2</v>
@@ -4315,7 +4309,7 @@
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B321" s="1">
         <v>0.31269066161846298</v>
@@ -4323,7 +4317,7 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B322" s="1">
         <v>1</v>
@@ -4331,7 +4325,7 @@
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B323" s="1">
         <v>-0.73203602206644502</v>
@@ -4339,7 +4333,7 @@
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B324" s="1">
         <v>-0.32943451798444301</v>
@@ -4347,7 +4341,7 @@
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B325" s="1">
         <v>-0.79900342900605303</v>
@@ -4355,7 +4349,7 @@
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B326" s="1">
         <v>-0.85532184793641497</v>
@@ -4363,7 +4357,7 @@
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B327" s="1">
         <v>-2.0375492809285099E-2</v>
@@ -4371,7 +4365,7 @@
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B328" s="1">
         <v>-0.26980740630913802</v>
@@ -4379,7 +4373,7 @@
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B329" s="1">
         <v>-0.24894008834490999</v>
@@ -4387,7 +4381,7 @@
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B330" s="1">
         <v>-0.56881596266378898</v>
@@ -4395,7 +4389,7 @@
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B331" s="1">
         <v>-0.85387131344132094</v>
@@ -4403,7 +4397,7 @@
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B332" s="1">
         <v>-0.34706964314356098</v>
@@ -4411,7 +4405,7 @@
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B333" s="1">
         <v>-0.51997460387491901</v>
@@ -4419,7 +4413,7 @@
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B334" s="1">
         <v>-1</v>
@@ -4427,7 +4421,7 @@
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B335" s="1">
         <v>0.23910044268320499</v>
@@ -4435,7 +4429,7 @@
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B336" s="1">
         <v>-0.92327125330412796</v>
@@ -4443,7 +4437,7 @@
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B337" s="1">
         <v>1</v>
@@ -4451,7 +4445,7 @@
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B338" s="1">
         <v>-0.93897474039557705</v>
@@ -4459,7 +4453,7 @@
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B339" s="1">
         <v>-0.52943332197857695</v>
@@ -4467,7 +4461,7 @@
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B340" s="1">
         <v>-0.47639772920626999</v>
@@ -4475,7 +4469,7 @@
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B341" s="1">
         <v>-0.102060621113889</v>
@@ -4483,7 +4477,7 @@
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B342" s="1">
         <v>-0.14612337591035099</v>
@@ -4491,7 +4485,7 @@
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B343" s="1">
         <v>-0.65821665818376396</v>
@@ -4499,7 +4493,7 @@
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B344" s="1">
         <v>-0.73972327653525105</v>
@@ -4507,7 +4501,7 @@
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B345" s="1">
         <v>0.32370102368247</v>
@@ -4515,7 +4509,7 @@
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B346" s="1">
         <v>-0.328606165631674</v>
@@ -4523,7 +4517,7 @@
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B347" s="1">
         <v>-0.158207571976481</v>
@@ -4531,7 +4525,7 @@
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B348" s="1">
         <v>-0.57033469793259395</v>
@@ -4539,7 +4533,7 @@
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B349" s="1">
         <v>-8.0105381014648105E-2</v>
@@ -4547,7 +4541,7 @@
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B350" s="1">
         <v>-0.49407163088327</v>
@@ -4555,7 +4549,7 @@
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B351" s="1">
         <v>-0.64427882310473406</v>
@@ -4563,7 +4557,7 @@
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B352" s="1">
         <v>-0.22882214864428399</v>
@@ -4571,7 +4565,7 @@
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B353" s="1">
         <v>-0.425904161105774</v>
@@ -4579,7 +4573,7 @@
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B354" s="1">
         <v>-0.76841784161932503</v>
@@ -4587,7 +4581,7 @@
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B355" s="1">
         <v>-0.42234386156684101</v>
@@ -4595,7 +4589,7 @@
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B356" s="1">
         <v>-0.80102477657140003</v>
@@ -4603,7 +4597,7 @@
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B357" s="1">
         <v>-0.20237795278638199</v>
@@ -4611,7 +4605,7 @@
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B358" s="1">
         <v>-0.55049050215696405</v>
@@ -4619,7 +4613,7 @@
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B359" s="1">
         <v>-0.50302168591076801</v>
@@ -4627,7 +4621,7 @@
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B360" s="1">
         <v>-0.66136951376103503</v>
@@ -4635,7 +4629,7 @@
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B361" s="1">
         <v>-0.39840281810045097</v>
@@ -4643,7 +4637,7 @@
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B362" s="1">
         <v>-0.44394127957018698</v>
@@ -4651,7 +4645,7 @@
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B363" s="1">
         <v>-0.392079184513274</v>
@@ -4659,7 +4653,7 @@
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B364" s="1">
         <v>-0.82985256297629095</v>
@@ -4667,7 +4661,7 @@
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B365" s="1">
         <v>-0.63138156970907</v>
@@ -4675,7 +4669,7 @@
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B366" s="1">
         <v>-0.34355204367939002</v>
@@ -4683,7 +4677,7 @@
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B367" s="1">
         <v>-0.48973577509798599</v>
@@ -4691,7 +4685,7 @@
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B368" s="1">
         <v>-1</v>
@@ -4699,7 +4693,7 @@
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B369" s="1">
         <v>-0.37927121095595401</v>
@@ -4707,7 +4701,7 @@
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B370" s="1">
         <v>-1.8090106505527E-2</v>
@@ -4715,7 +4709,7 @@
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B371" s="1">
         <v>-0.55961225410382298</v>
@@ -4723,7 +4717,7 @@
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B372" s="1">
         <v>-1</v>
@@ -4731,7 +4725,7 @@
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B373" s="1">
         <v>-0.33755433645062199</v>
@@ -4739,7 +4733,7 @@
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B374" s="1">
         <v>-0.53097008103654697</v>
@@ -4747,7 +4741,7 @@
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B375" s="1">
         <v>-0.50993885782241799</v>
@@ -4755,7 +4749,7 @@
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B376" s="1">
         <v>-0.34742211018291302</v>
@@ -4763,7 +4757,7 @@
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B377" s="1">
         <v>-0.74847747834834499</v>
@@ -4771,7 +4765,7 @@
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B378" s="1">
         <v>-0.71604564698989703</v>
@@ -4779,7 +4773,7 @@
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B379" s="1">
         <v>-0.86772394774946104</v>
@@ -4787,7 +4781,7 @@
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B380" s="1">
         <v>-0.31354481346039198</v>
@@ -4795,7 +4789,7 @@
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B381" s="1">
         <v>-0.43109669374908899</v>
@@ -4803,7 +4797,7 @@
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B382" s="1">
         <v>-0.33373421310042201</v>
@@ -4811,7 +4805,7 @@
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B383" s="1">
         <v>-0.54669478045099695</v>
@@ -4819,7 +4813,7 @@
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B384" s="1">
         <v>-0.33300811233277799</v>
@@ -4827,7 +4821,7 @@
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B385" s="1">
         <v>3.02438921592296E-2</v>
@@ -4835,7 +4829,7 @@
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B386" s="1">
         <v>-0.65246210619865996</v>
@@ -4843,7 +4837,7 @@
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B387" s="1">
         <v>-0.68397350616991504</v>
@@ -4851,7 +4845,7 @@
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B388" s="1">
         <v>-0.59643754531774196</v>
@@ -4859,7 +4853,7 @@
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B389" s="1">
         <v>4.6937132134900798E-2</v>
@@ -4867,7 +4861,7 @@
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B390" s="1">
         <v>-0.45017772758270402</v>
@@ -4875,7 +4869,7 @@
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B391" s="1">
         <v>-0.538351542995399</v>
@@ -4883,7 +4877,7 @@
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B392" s="1">
         <v>-0.54950338954695299</v>
@@ -4891,7 +4885,7 @@
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B393" s="1">
         <v>-0.83230897564945405</v>
@@ -4899,7 +4893,7 @@
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B394" s="1">
         <v>-0.57644203493206803</v>
@@ -4907,7 +4901,7 @@
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B395" s="1">
         <v>-0.65707896653763198</v>
@@ -4915,7 +4909,7 @@
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B396" s="1">
         <v>-0.81092597901001195</v>
@@ -4923,7 +4917,7 @@
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B397" s="1">
         <v>-0.644302322136314</v>
@@ -4931,7 +4925,7 @@
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A398" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B398" s="1">
         <v>-0.46187558000375101</v>
@@ -4939,7 +4933,7 @@
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B399" s="1">
         <v>-6.4296443263401198E-2</v>
@@ -4947,7 +4941,7 @@
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B400" s="1">
         <v>-0.40971231176882</v>
@@ -4955,7 +4949,7 @@
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B401" s="1">
         <v>-3.5838441281391797E-2</v>
@@ -4963,7 +4957,7 @@
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A402" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B402" s="1">
         <v>-0.82063922999619399</v>
@@ -4971,7 +4965,7 @@
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B403" s="1">
         <v>-0.82461656680074003</v>
@@ -4979,7 +4973,7 @@
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B404" s="1">
         <v>0.23374514608029501</v>
@@ -4987,7 +4981,7 @@
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B405" s="1">
         <v>-0.38604435312959801</v>
@@ -4995,7 +4989,7 @@
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B406" s="1">
         <v>-0.56825013845573402</v>
@@ -5003,7 +4997,7 @@
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B407" s="1">
         <v>-0.533709480532225</v>
@@ -5011,7 +5005,7 @@
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A408" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B408" s="1">
         <v>-0.395330240814185</v>
@@ -5019,7 +5013,7 @@
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A409" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B409" s="1">
         <v>-0.20530686634428</v>
@@ -5027,7 +5021,7 @@
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A410" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B410" s="1">
         <v>-0.25961585972864298</v>
@@ -5035,7 +5029,7 @@
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B411" s="1">
         <v>-0.23667735965445499</v>
@@ -5043,7 +5037,7 @@
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B412" s="1">
         <v>-0.42706105350742701</v>
@@ -5051,7 +5045,7 @@
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B413" s="1">
         <v>-0.37421851283053598</v>
@@ -5059,7 +5053,7 @@
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B414" s="1">
         <v>-0.82149506768129299</v>
@@ -5067,7 +5061,7 @@
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B415" s="1">
         <v>-0.121696663544779</v>
@@ -5075,7 +5069,7 @@
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B416" s="1">
         <v>-0.87312891110829505</v>
@@ -5083,7 +5077,7 @@
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A417" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B417" s="1">
         <v>-0.59243697232345105</v>
@@ -5091,7 +5085,7 @@
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B418" s="1">
         <v>-0.732489286852543</v>
@@ -5099,7 +5093,7 @@
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A419" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B419" s="1">
         <v>-0.18183939945782801</v>
@@ -5107,7 +5101,7 @@
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A420" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B420" s="1">
         <v>-0.55085686947745305</v>
@@ -5115,7 +5109,7 @@
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B421" s="1">
         <v>-0.42498897641406902</v>
@@ -5123,7 +5117,7 @@
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B422" s="1">
         <v>-0.32761768654358298</v>
@@ -5131,7 +5125,7 @@
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A423" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B423" s="1">
         <v>-0.96120884464271505</v>
@@ -5139,7 +5133,7 @@
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A424" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B424" s="1">
         <v>-0.62692915179099495</v>
@@ -5147,7 +5141,7 @@
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A425" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B425" s="1">
         <v>-0.179822668756702</v>
@@ -5155,7 +5149,7 @@
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A426" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B426" s="1">
         <v>-0.36325329863674599</v>
@@ -5163,7 +5157,7 @@
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B427" s="1">
         <v>-0.75189890511254298</v>
@@ -5171,7 +5165,7 @@
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B428" s="1">
         <v>-0.72332713459604303</v>
@@ -5179,7 +5173,7 @@
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A429" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B429" s="1">
         <v>-0.38545787516754698</v>
@@ -5187,7 +5181,7 @@
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A430" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B430" s="1">
         <v>0.179685064857355</v>
@@ -5195,7 +5189,7 @@
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A431" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B431" s="1">
         <v>8.7294614934849399E-2</v>
@@ -5203,7 +5197,7 @@
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A432" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B432" s="1">
         <v>-0.25812249019419897</v>
@@ -5211,7 +5205,7 @@
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A433" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B433" s="1">
         <v>-0.72995702962259501</v>
@@ -5219,7 +5213,7 @@
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A434" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B434" s="1">
         <v>-0.71843222238385196</v>
@@ -5227,7 +5221,7 @@
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A435" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B435" s="1">
         <v>-0.91055983180439404</v>
@@ -5235,7 +5229,7 @@
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A436" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B436" s="1">
         <v>-0.111131501787316</v>
@@ -5243,7 +5237,7 @@
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A437" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B437" s="1">
         <v>-0.37018641206715902</v>
@@ -5251,7 +5245,7 @@
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A438" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B438" s="1">
         <v>-0.62485411150986703</v>
@@ -5259,7 +5253,7 @@
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A439" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B439" s="1">
         <v>-0.56242423556973398</v>
@@ -5267,7 +5261,7 @@
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A440" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B440" s="1">
         <v>-0.76498445154019601</v>
@@ -5275,7 +5269,7 @@
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A441" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B441" s="1">
         <v>-0.92478732222503701</v>
@@ -5283,7 +5277,7 @@
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A442" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B442" s="1">
         <v>-0.89341937869940802</v>
@@ -5291,7 +5285,7 @@
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A443" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B443" s="1">
         <v>-0.27677071566417499</v>
@@ -5299,7 +5293,7 @@
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A444" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B444" s="1">
         <v>0.82856191107670396</v>
@@ -5307,7 +5301,7 @@
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A445" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B445" s="1">
         <v>-0.75804460280354202</v>
@@ -5315,7 +5309,7 @@
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A446" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B446" s="1">
         <v>-0.72102744580282396</v>
@@ -5323,7 +5317,7 @@
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A447" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B447" s="1">
         <v>-0.37649418953932901</v>
@@ -5331,7 +5325,7 @@
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A448" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B448" s="1">
         <v>-0.29251426222098598</v>
@@ -5339,7 +5333,7 @@
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A449" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B449" s="1">
         <v>-0.25449777307424198</v>
@@ -5347,7 +5341,7 @@
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A450" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B450" s="1">
         <v>-0.29206322426282999</v>
@@ -5355,14 +5349,14 @@
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A451" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B451" s="1">
         <v>6.37198449751228E-2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B451">
+  <sortState ref="A2:B451">
     <sortCondition ref="A1:A451"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>